<commit_message>
Added methods for read/write cars. Added first row and cell in sheets 3 and 4 set to 1. Must be set to 1 in order to find next row to read/write from. Refers to #21.
</commit_message>
<xml_diff>
--- a/TrafficSimulator/data.xlsx
+++ b/TrafficSimulator/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="720" windowWidth="13665" windowHeight="10845"/>
+    <workbookView xWindow="14295" yWindow="720" windowWidth="13665" windowHeight="10845" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -432,8 +433,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -578,7 +579,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -613,7 +613,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -789,14 +788,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+    <sheetView topLeftCell="A220" workbookViewId="0">
       <selection activeCell="I1" sqref="I1:I236"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="3.28515625" customWidth="1"/>
@@ -807,7 +806,7 @@
     <col min="7" max="7" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="16.5" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -836,7 +835,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="16.5" thickBot="1">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -865,7 +864,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="16.5" thickBot="1">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -894,7 +893,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="16.5" thickBot="1">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -923,7 +922,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="16.5" thickBot="1">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -952,7 +951,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="16.5" thickBot="1">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -981,7 +980,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="16.5" thickBot="1">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1010,7 +1009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="16.5" thickBot="1">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1039,7 +1038,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="16.5" thickBot="1">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1068,7 +1067,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="16.5" thickBot="1">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1097,7 +1096,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="16.5" thickBot="1">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1126,7 +1125,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="16.5" thickBot="1">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1155,7 +1154,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="16.5" thickBot="1">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1184,7 +1183,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="16.5" thickBot="1">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1213,7 +1212,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="16.5" thickBot="1">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1242,7 +1241,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="16.5" thickBot="1">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1271,7 +1270,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="16.5" thickBot="1">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1300,7 +1299,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="16.5" thickBot="1">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1329,7 +1328,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="16.5" thickBot="1">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1358,7 +1357,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="16.5" thickBot="1">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1387,7 +1386,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="16.5" thickBot="1">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1416,7 +1415,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="16.5" thickBot="1">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1445,7 +1444,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="16.5" thickBot="1">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1474,7 +1473,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="16.5" thickBot="1">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1503,7 +1502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="16.5" thickBot="1">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1532,7 +1531,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="16.5" thickBot="1">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1561,7 +1560,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="16.5" thickBot="1">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1590,7 +1589,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="16.5" thickBot="1">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1619,7 +1618,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="16.5" thickBot="1">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -1648,7 +1647,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="16.5" thickBot="1">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1677,7 +1676,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="16.5" thickBot="1">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1706,7 +1705,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="16.5" thickBot="1">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -1735,7 +1734,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="16.5" thickBot="1">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -1764,7 +1763,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="16.5" thickBot="1">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1793,7 +1792,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="16.5" thickBot="1">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -1822,7 +1821,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="16.5" thickBot="1">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -1851,7 +1850,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="16.5" thickBot="1">
       <c r="A37" t="s">
         <v>19</v>
       </c>
@@ -1880,7 +1879,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="16.5" thickBot="1">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -1909,7 +1908,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="16.5" thickBot="1">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -1938,7 +1937,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="16.5" thickBot="1">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -1967,7 +1966,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="16.5" thickBot="1">
       <c r="A41" t="s">
         <v>23</v>
       </c>
@@ -1996,7 +1995,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="16.5" thickBot="1">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -2025,7 +2024,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="16.5" thickBot="1">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -2054,7 +2053,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="16.5" thickBot="1">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -2083,7 +2082,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="16.5" thickBot="1">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -2112,7 +2111,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="16.5" thickBot="1">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -2141,7 +2140,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="16.5" thickBot="1">
       <c r="A47" t="s">
         <v>28</v>
       </c>
@@ -2170,7 +2169,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="16.5" thickBot="1">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -2199,7 +2198,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="16.5" thickBot="1">
       <c r="A49" t="s">
         <v>29</v>
       </c>
@@ -2228,7 +2227,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="16.5" thickBot="1">
       <c r="A50" t="s">
         <v>29</v>
       </c>
@@ -2257,7 +2256,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="16.5" thickBot="1">
       <c r="A51" t="s">
         <v>35</v>
       </c>
@@ -2286,7 +2285,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="16.5" thickBot="1">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -2315,7 +2314,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="16.5" thickBot="1">
       <c r="A53" t="s">
         <v>37</v>
       </c>
@@ -2344,7 +2343,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="16.5" thickBot="1">
       <c r="A54" t="s">
         <v>40</v>
       </c>
@@ -2373,7 +2372,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="16.5" thickBot="1">
       <c r="A55" t="s">
         <v>40</v>
       </c>
@@ -2402,7 +2401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="16.5" thickBot="1">
       <c r="A56" t="s">
         <v>40</v>
       </c>
@@ -2431,7 +2430,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="16.5" thickBot="1">
       <c r="A57" t="s">
         <v>30</v>
       </c>
@@ -2460,7 +2459,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="16.5" thickBot="1">
       <c r="A58" t="s">
         <v>30</v>
       </c>
@@ -2489,7 +2488,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="16.5" thickBot="1">
       <c r="A59" t="s">
         <v>30</v>
       </c>
@@ -2518,7 +2517,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="16.5" thickBot="1">
       <c r="A60" t="s">
         <v>30</v>
       </c>
@@ -2547,7 +2546,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="16.5" thickBot="1">
       <c r="A61" t="s">
         <v>31</v>
       </c>
@@ -2576,7 +2575,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="16.5" thickBot="1">
       <c r="A62" t="s">
         <v>31</v>
       </c>
@@ -2605,7 +2604,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="16.5" thickBot="1">
       <c r="A63" t="s">
         <v>31</v>
       </c>
@@ -2634,7 +2633,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="16.5" thickBot="1">
       <c r="A64" t="s">
         <v>31</v>
       </c>
@@ -2663,7 +2662,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="16.5" thickBot="1">
       <c r="A65" t="s">
         <v>46</v>
       </c>
@@ -2692,7 +2691,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="16.5" thickBot="1">
       <c r="A66" t="s">
         <v>46</v>
       </c>
@@ -2721,7 +2720,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="16.5" thickBot="1">
       <c r="A67" t="s">
         <v>46</v>
       </c>
@@ -2750,7 +2749,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="16.5" thickBot="1">
       <c r="A68" t="s">
         <v>49</v>
       </c>
@@ -2779,7 +2778,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="16.5" thickBot="1">
       <c r="A69" t="s">
         <v>49</v>
       </c>
@@ -2808,7 +2807,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="16.5" thickBot="1">
       <c r="A70" t="s">
         <v>49</v>
       </c>
@@ -2837,7 +2836,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="16.5" thickBot="1">
       <c r="A71" t="s">
         <v>52</v>
       </c>
@@ -2866,7 +2865,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="16.5" thickBot="1">
       <c r="A72" t="s">
         <v>52</v>
       </c>
@@ -2895,7 +2894,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="16.5" thickBot="1">
       <c r="A73" t="s">
         <v>52</v>
       </c>
@@ -2924,7 +2923,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="16.5" thickBot="1">
       <c r="A74" t="s">
         <v>55</v>
       </c>
@@ -2953,7 +2952,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="16.5" thickBot="1">
       <c r="A75" t="s">
         <v>55</v>
       </c>
@@ -2982,7 +2981,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="16.5" thickBot="1">
       <c r="A76" t="s">
         <v>32</v>
       </c>
@@ -3011,7 +3010,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="16.5" thickBot="1">
       <c r="A77" t="s">
         <v>32</v>
       </c>
@@ -3040,7 +3039,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="16.5" thickBot="1">
       <c r="A78" t="s">
         <v>32</v>
       </c>
@@ -3069,7 +3068,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="16.5" thickBot="1">
       <c r="A79" t="s">
         <v>47</v>
       </c>
@@ -3098,7 +3097,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" ht="16.5" thickBot="1">
       <c r="A80" t="s">
         <v>47</v>
       </c>
@@ -3127,7 +3126,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" ht="16.5" thickBot="1">
       <c r="A81" t="s">
         <v>47</v>
       </c>
@@ -3156,7 +3155,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="16.5" thickBot="1">
       <c r="A82" t="s">
         <v>50</v>
       </c>
@@ -3185,7 +3184,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="16.5" thickBot="1">
       <c r="A83" t="s">
         <v>50</v>
       </c>
@@ -3214,7 +3213,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="16.5" thickBot="1">
       <c r="A84" t="s">
         <v>50</v>
       </c>
@@ -3243,7 +3242,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" ht="16.5" thickBot="1">
       <c r="A85" t="s">
         <v>50</v>
       </c>
@@ -3272,7 +3271,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="16.5" thickBot="1">
       <c r="A86" t="s">
         <v>53</v>
       </c>
@@ -3301,7 +3300,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="16.5" thickBot="1">
       <c r="A87" t="s">
         <v>53</v>
       </c>
@@ -3330,7 +3329,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="16.5" thickBot="1">
       <c r="A88" t="s">
         <v>53</v>
       </c>
@@ -3359,7 +3358,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="16.5" thickBot="1">
       <c r="A89" t="s">
         <v>60</v>
       </c>
@@ -3388,7 +3387,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="16.5" thickBot="1">
       <c r="A90" t="s">
         <v>60</v>
       </c>
@@ -3417,7 +3416,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" ht="16.5" thickBot="1">
       <c r="A91" t="s">
         <v>60</v>
       </c>
@@ -3446,7 +3445,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" ht="16.5" thickBot="1">
       <c r="A92" t="s">
         <v>56</v>
       </c>
@@ -3475,7 +3474,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" ht="16.5" thickBot="1">
       <c r="A93" t="s">
         <v>56</v>
       </c>
@@ -3504,7 +3503,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="16.5" thickBot="1">
       <c r="A94" t="s">
         <v>56</v>
       </c>
@@ -3533,7 +3532,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="16.5" thickBot="1">
       <c r="A95" t="s">
         <v>38</v>
       </c>
@@ -3562,7 +3561,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="16.5" thickBot="1">
       <c r="A96" t="s">
         <v>38</v>
       </c>
@@ -3591,7 +3590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" ht="16.5" thickBot="1">
       <c r="A97" t="s">
         <v>38</v>
       </c>
@@ -3620,7 +3619,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" ht="16.5" thickBot="1">
       <c r="A98" t="s">
         <v>42</v>
       </c>
@@ -3649,7 +3648,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" ht="16.5" thickBot="1">
       <c r="A99" t="s">
         <v>42</v>
       </c>
@@ -3678,7 +3677,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" ht="16.5" thickBot="1">
       <c r="A100" t="s">
         <v>42</v>
       </c>
@@ -3707,7 +3706,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" ht="16.5" thickBot="1">
       <c r="A101" t="s">
         <v>42</v>
       </c>
@@ -3736,7 +3735,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" ht="16.5" thickBot="1">
       <c r="A102" t="s">
         <v>44</v>
       </c>
@@ -3765,7 +3764,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" ht="16.5" thickBot="1">
       <c r="A103" t="s">
         <v>44</v>
       </c>
@@ -3794,7 +3793,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" ht="16.5" thickBot="1">
       <c r="A104" t="s">
         <v>44</v>
       </c>
@@ -3823,7 +3822,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" ht="16.5" thickBot="1">
       <c r="A105" t="s">
         <v>44</v>
       </c>
@@ -3852,7 +3851,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" ht="16.5" thickBot="1">
       <c r="A106" t="s">
         <v>69</v>
       </c>
@@ -3881,7 +3880,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" ht="16.5" thickBot="1">
       <c r="A107" t="s">
         <v>69</v>
       </c>
@@ -3910,7 +3909,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" ht="16.5" thickBot="1">
       <c r="A108" t="s">
         <v>45</v>
       </c>
@@ -3939,7 +3938,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" ht="16.5" thickBot="1">
       <c r="A109" t="s">
         <v>45</v>
       </c>
@@ -3968,7 +3967,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" ht="16.5" thickBot="1">
       <c r="A110" t="s">
         <v>45</v>
       </c>
@@ -3997,7 +3996,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" ht="16.5" thickBot="1">
       <c r="A111" t="s">
         <v>45</v>
       </c>
@@ -4026,7 +4025,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" ht="16.5" thickBot="1">
       <c r="A112" t="s">
         <v>57</v>
       </c>
@@ -4055,7 +4054,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" ht="16.5" thickBot="1">
       <c r="A113" t="s">
         <v>57</v>
       </c>
@@ -4084,7 +4083,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" ht="16.5" thickBot="1">
       <c r="A114" t="s">
         <v>57</v>
       </c>
@@ -4113,7 +4112,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" ht="16.5" thickBot="1">
       <c r="A115" t="s">
         <v>63</v>
       </c>
@@ -4142,7 +4141,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" ht="16.5" thickBot="1">
       <c r="A116" t="s">
         <v>63</v>
       </c>
@@ -4171,7 +4170,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" ht="16.5" thickBot="1">
       <c r="A117" t="s">
         <v>63</v>
       </c>
@@ -4200,7 +4199,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" ht="16.5" thickBot="1">
       <c r="A118" t="s">
         <v>73</v>
       </c>
@@ -4229,7 +4228,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" ht="16.5" thickBot="1">
       <c r="A119" t="s">
         <v>75</v>
       </c>
@@ -4258,7 +4257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" ht="16.5" thickBot="1">
       <c r="A120" t="s">
         <v>64</v>
       </c>
@@ -4287,7 +4286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="16.5" thickBot="1">
       <c r="A121" t="s">
         <v>64</v>
       </c>
@@ -4316,7 +4315,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" ht="16.5" thickBot="1">
       <c r="A122" t="s">
         <v>64</v>
       </c>
@@ -4345,7 +4344,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" ht="16.5" thickBot="1">
       <c r="A123" t="s">
         <v>71</v>
       </c>
@@ -4374,7 +4373,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" ht="16.5" thickBot="1">
       <c r="A124" t="s">
         <v>71</v>
       </c>
@@ -4403,7 +4402,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" ht="16.5" thickBot="1">
       <c r="A125" t="s">
         <v>71</v>
       </c>
@@ -4432,7 +4431,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" ht="16.5" thickBot="1">
       <c r="A126" t="s">
         <v>59</v>
       </c>
@@ -4461,7 +4460,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" ht="16.5" thickBot="1">
       <c r="A127" t="s">
         <v>59</v>
       </c>
@@ -4490,7 +4489,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" ht="16.5" thickBot="1">
       <c r="A128" t="s">
         <v>59</v>
       </c>
@@ -4519,7 +4518,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" ht="16.5" thickBot="1">
       <c r="A129" t="s">
         <v>59</v>
       </c>
@@ -4548,7 +4547,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" ht="16.5" thickBot="1">
       <c r="A130" t="s">
         <v>61</v>
       </c>
@@ -4577,7 +4576,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" ht="16.5" thickBot="1">
       <c r="A131" t="s">
         <v>61</v>
       </c>
@@ -4606,7 +4605,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" ht="16.5" thickBot="1">
       <c r="A132" t="s">
         <v>61</v>
       </c>
@@ -4635,7 +4634,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" ht="16.5" thickBot="1">
       <c r="A133" t="s">
         <v>61</v>
       </c>
@@ -4664,7 +4663,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" ht="16.5" thickBot="1">
       <c r="A134" t="s">
         <v>72</v>
       </c>
@@ -4693,7 +4692,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" ht="16.5" thickBot="1">
       <c r="A135" t="s">
         <v>72</v>
       </c>
@@ -4722,7 +4721,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" ht="16.5" thickBot="1">
       <c r="A136" t="s">
         <v>72</v>
       </c>
@@ -4751,7 +4750,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" ht="16.5" thickBot="1">
       <c r="A137" t="s">
         <v>72</v>
       </c>
@@ -4780,7 +4779,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" ht="16.5" thickBot="1">
       <c r="A138" t="s">
         <v>84</v>
       </c>
@@ -4809,7 +4808,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" ht="16.5" thickBot="1">
       <c r="A139" t="s">
         <v>84</v>
       </c>
@@ -4838,7 +4837,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" ht="16.5" thickBot="1">
       <c r="A140" t="s">
         <v>84</v>
       </c>
@@ -4867,7 +4866,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" ht="16.5" thickBot="1">
       <c r="A141" t="s">
         <v>87</v>
       </c>
@@ -4896,7 +4895,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" ht="16.5" thickBot="1">
       <c r="A142" t="s">
         <v>77</v>
       </c>
@@ -4925,7 +4924,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" ht="16.5" thickBot="1">
       <c r="A143" t="s">
         <v>77</v>
       </c>
@@ -4954,7 +4953,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" ht="16.5" thickBot="1">
       <c r="A144" t="s">
         <v>77</v>
       </c>
@@ -4983,7 +4982,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" ht="16.5" thickBot="1">
       <c r="A145" t="s">
         <v>79</v>
       </c>
@@ -5012,7 +5011,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="146" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" ht="16.5" thickBot="1">
       <c r="A146" t="s">
         <v>79</v>
       </c>
@@ -5041,7 +5040,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="147" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" ht="16.5" thickBot="1">
       <c r="A147" t="s">
         <v>79</v>
       </c>
@@ -5070,7 +5069,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" ht="16.5" thickBot="1">
       <c r="A148" t="s">
         <v>70</v>
       </c>
@@ -5099,7 +5098,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" ht="16.5" thickBot="1">
       <c r="A149" t="s">
         <v>70</v>
       </c>
@@ -5128,7 +5127,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" ht="16.5" thickBot="1">
       <c r="A150" t="s">
         <v>70</v>
       </c>
@@ -5157,7 +5156,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="151" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" ht="16.5" thickBot="1">
       <c r="A151" t="s">
         <v>92</v>
       </c>
@@ -5186,7 +5185,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" ht="16.5" thickBot="1">
       <c r="A152" t="s">
         <v>92</v>
       </c>
@@ -5215,7 +5214,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="153" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" ht="16.5" thickBot="1">
       <c r="A153" t="s">
         <v>92</v>
       </c>
@@ -5244,7 +5243,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="154" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" ht="16.5" thickBot="1">
       <c r="A154" t="s">
         <v>88</v>
       </c>
@@ -5273,7 +5272,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" ht="16.5" thickBot="1">
       <c r="A155" t="s">
         <v>88</v>
       </c>
@@ -5302,7 +5301,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="156" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" ht="16.5" thickBot="1">
       <c r="A156" t="s">
         <v>88</v>
       </c>
@@ -5331,7 +5330,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" ht="16.5" thickBot="1">
       <c r="A157" t="s">
         <v>88</v>
       </c>
@@ -5360,7 +5359,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" ht="16.5" thickBot="1">
       <c r="A158" t="s">
         <v>90</v>
       </c>
@@ -5389,7 +5388,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="159" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" ht="16.5" thickBot="1">
       <c r="A159" t="s">
         <v>90</v>
       </c>
@@ -5418,7 +5417,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="160" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" ht="16.5" thickBot="1">
       <c r="A160" t="s">
         <v>90</v>
       </c>
@@ -5447,7 +5446,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="161" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" ht="16.5" thickBot="1">
       <c r="A161" t="s">
         <v>90</v>
       </c>
@@ -5476,7 +5475,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="162" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" ht="16.5" thickBot="1">
       <c r="A162" t="s">
         <v>80</v>
       </c>
@@ -5505,7 +5504,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="163" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" ht="16.5" thickBot="1">
       <c r="A163" t="s">
         <v>80</v>
       </c>
@@ -5534,7 +5533,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="164" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" ht="16.5" thickBot="1">
       <c r="A164" t="s">
         <v>80</v>
       </c>
@@ -5563,7 +5562,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="165" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" ht="16.5" thickBot="1">
       <c r="A165" t="s">
         <v>80</v>
       </c>
@@ -5592,7 +5591,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" ht="16.5" thickBot="1">
       <c r="A166" t="s">
         <v>82</v>
       </c>
@@ -5621,7 +5620,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="167" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" ht="16.5" thickBot="1">
       <c r="A167" t="s">
         <v>82</v>
       </c>
@@ -5650,7 +5649,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="168" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" ht="16.5" thickBot="1">
       <c r="A168" t="s">
         <v>82</v>
       </c>
@@ -5679,7 +5678,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" ht="16.5" thickBot="1">
       <c r="A169" t="s">
         <v>82</v>
       </c>
@@ -5708,7 +5707,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="170" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" ht="16.5" thickBot="1">
       <c r="A170" t="s">
         <v>85</v>
       </c>
@@ -5737,7 +5736,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="171" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" ht="16.5" thickBot="1">
       <c r="A171" t="s">
         <v>98</v>
       </c>
@@ -5766,7 +5765,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" ht="16.5" thickBot="1">
       <c r="A172" t="s">
         <v>98</v>
       </c>
@@ -5795,7 +5794,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="173" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" ht="16.5" thickBot="1">
       <c r="A173" t="s">
         <v>67</v>
       </c>
@@ -5824,7 +5823,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="174" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" ht="16.5" thickBot="1">
       <c r="A174" t="s">
         <v>67</v>
       </c>
@@ -5853,7 +5852,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" ht="16.5" thickBot="1">
       <c r="A175" t="s">
         <v>67</v>
       </c>
@@ -5882,7 +5881,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="176" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9" ht="16.5" thickBot="1">
       <c r="A176" t="s">
         <v>91</v>
       </c>
@@ -5911,7 +5910,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="177" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" ht="16.5" thickBot="1">
       <c r="A177" t="s">
         <v>91</v>
       </c>
@@ -5940,7 +5939,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="178" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" ht="16.5" thickBot="1">
       <c r="A178" t="s">
         <v>91</v>
       </c>
@@ -5969,7 +5968,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="179" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" ht="16.5" thickBot="1">
       <c r="A179" t="s">
         <v>91</v>
       </c>
@@ -5998,7 +5997,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="180" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" ht="16.5" thickBot="1">
       <c r="A180" t="s">
         <v>94</v>
       </c>
@@ -6027,7 +6026,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="181" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" ht="16.5" thickBot="1">
       <c r="A181" t="s">
         <v>94</v>
       </c>
@@ -6056,7 +6055,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="182" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" ht="16.5" thickBot="1">
       <c r="A182" t="s">
         <v>94</v>
       </c>
@@ -6085,7 +6084,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="183" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" ht="16.5" thickBot="1">
       <c r="A183" t="s">
         <v>105</v>
       </c>
@@ -6114,7 +6113,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="184" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" ht="16.5" thickBot="1">
       <c r="A184" t="s">
         <v>105</v>
       </c>
@@ -6143,7 +6142,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" ht="16.5" thickBot="1">
       <c r="A185" t="s">
         <v>105</v>
       </c>
@@ -6172,7 +6171,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="186" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" ht="16.5" thickBot="1">
       <c r="A186" t="s">
         <v>96</v>
       </c>
@@ -6201,7 +6200,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="187" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" ht="16.5" thickBot="1">
       <c r="A187" t="s">
         <v>96</v>
       </c>
@@ -6230,7 +6229,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="188" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" ht="16.5" thickBot="1">
       <c r="A188" t="s">
         <v>96</v>
       </c>
@@ -6259,7 +6258,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="189" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" ht="16.5" thickBot="1">
       <c r="A189" t="s">
         <v>96</v>
       </c>
@@ -6288,7 +6287,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="190" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" ht="16.5" thickBot="1">
       <c r="A190" t="s">
         <v>97</v>
       </c>
@@ -6317,7 +6316,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="191" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" ht="16.5" thickBot="1">
       <c r="A191" t="s">
         <v>97</v>
       </c>
@@ -6346,7 +6345,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="192" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" ht="16.5" thickBot="1">
       <c r="A192" t="s">
         <v>97</v>
       </c>
@@ -6375,7 +6374,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="193" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" ht="16.5" thickBot="1">
       <c r="A193" t="s">
         <v>97</v>
       </c>
@@ -6404,7 +6403,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" ht="16.5" thickBot="1">
       <c r="A194" t="s">
         <v>108</v>
       </c>
@@ -6433,7 +6432,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="195" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" ht="16.5" thickBot="1">
       <c r="A195" t="s">
         <v>108</v>
       </c>
@@ -6462,7 +6461,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" ht="16.5" thickBot="1">
       <c r="A196" t="s">
         <v>108</v>
       </c>
@@ -6491,7 +6490,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" ht="16.5" thickBot="1">
       <c r="A197" t="s">
         <v>99</v>
       </c>
@@ -6520,7 +6519,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="198" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" ht="16.5" thickBot="1">
       <c r="A198" t="s">
         <v>99</v>
       </c>
@@ -6549,7 +6548,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" ht="16.5" thickBot="1">
       <c r="A199" t="s">
         <v>99</v>
       </c>
@@ -6578,7 +6577,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="200" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" ht="16.5" thickBot="1">
       <c r="A200" t="s">
         <v>111</v>
       </c>
@@ -6607,7 +6606,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="201" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" ht="16.5" thickBot="1">
       <c r="A201" t="s">
         <v>111</v>
       </c>
@@ -6636,7 +6635,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="202" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" ht="16.5" thickBot="1">
       <c r="A202" t="s">
         <v>111</v>
       </c>
@@ -6665,7 +6664,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="203" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" ht="16.5" thickBot="1">
       <c r="A203" t="s">
         <v>107</v>
       </c>
@@ -6694,7 +6693,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="204" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" ht="16.5" thickBot="1">
       <c r="A204" t="s">
         <v>107</v>
       </c>
@@ -6723,7 +6722,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="205" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" ht="16.5" thickBot="1">
       <c r="A205" t="s">
         <v>107</v>
       </c>
@@ -6752,7 +6751,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="206" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" ht="16.5" thickBot="1">
       <c r="A206" t="s">
         <v>110</v>
       </c>
@@ -6781,7 +6780,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="207" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" ht="16.5" thickBot="1">
       <c r="A207" t="s">
         <v>110</v>
       </c>
@@ -6810,7 +6809,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="208" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" ht="16.5" thickBot="1">
       <c r="A208" t="s">
         <v>110</v>
       </c>
@@ -6839,7 +6838,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:9" ht="16.5" thickBot="1">
       <c r="A209" t="s">
         <v>106</v>
       </c>
@@ -6868,7 +6867,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="210" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:9" ht="16.5" thickBot="1">
       <c r="A210" t="s">
         <v>106</v>
       </c>
@@ -6897,7 +6896,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="211" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:9" ht="16.5" thickBot="1">
       <c r="A211" t="s">
         <v>106</v>
       </c>
@@ -6926,7 +6925,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="212" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:9" ht="16.5" thickBot="1">
       <c r="A212" t="s">
         <v>106</v>
       </c>
@@ -6955,7 +6954,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="213" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9" ht="16.5" thickBot="1">
       <c r="A213" t="s">
         <v>115</v>
       </c>
@@ -6984,7 +6983,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="214" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9" ht="16.5" thickBot="1">
       <c r="A214" t="s">
         <v>115</v>
       </c>
@@ -7013,7 +7012,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="215" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9" ht="16.5" thickBot="1">
       <c r="A215" t="s">
         <v>115</v>
       </c>
@@ -7042,7 +7041,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:9" ht="16.5" thickBot="1">
       <c r="A216" t="s">
         <v>119</v>
       </c>
@@ -7071,7 +7070,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="217" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:9" ht="16.5" thickBot="1">
       <c r="A217" t="s">
         <v>100</v>
       </c>
@@ -7100,7 +7099,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="218" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:9" ht="16.5" thickBot="1">
       <c r="A218" t="s">
         <v>100</v>
       </c>
@@ -7129,7 +7128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:9" ht="16.5" thickBot="1">
       <c r="A219" t="s">
         <v>100</v>
       </c>
@@ -7158,7 +7157,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="220" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" ht="16.5" thickBot="1">
       <c r="A220" t="s">
         <v>102</v>
       </c>
@@ -7187,7 +7186,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="221" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9" ht="16.5" thickBot="1">
       <c r="A221" t="s">
         <v>102</v>
       </c>
@@ -7216,7 +7215,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" ht="16.5" thickBot="1">
       <c r="A222" t="s">
         <v>102</v>
       </c>
@@ -7245,7 +7244,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="223" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9" ht="16.5" thickBot="1">
       <c r="A223" t="s">
         <v>116</v>
       </c>
@@ -7274,7 +7273,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="224" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:9" ht="16.5" thickBot="1">
       <c r="A224" t="s">
         <v>116</v>
       </c>
@@ -7303,7 +7302,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="225" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" ht="16.5" thickBot="1">
       <c r="A225" t="s">
         <v>116</v>
       </c>
@@ -7332,7 +7331,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="226" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" ht="16.5" thickBot="1">
       <c r="A226" t="s">
         <v>118</v>
       </c>
@@ -7361,7 +7360,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="227" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" ht="16.5" thickBot="1">
       <c r="A227" t="s">
         <v>118</v>
       </c>
@@ -7390,7 +7389,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="228" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" ht="16.5" thickBot="1">
       <c r="A228" t="s">
         <v>118</v>
       </c>
@@ -7419,7 +7418,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" ht="16.5" thickBot="1">
       <c r="A229" t="s">
         <v>118</v>
       </c>
@@ -7448,7 +7447,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="230" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" ht="16.5" thickBot="1">
       <c r="A230" t="s">
         <v>113</v>
       </c>
@@ -7477,7 +7476,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="231" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9" ht="16.5" thickBot="1">
       <c r="A231" t="s">
         <v>113</v>
       </c>
@@ -7506,7 +7505,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="232" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9" ht="16.5" thickBot="1">
       <c r="A232" t="s">
         <v>113</v>
       </c>
@@ -7535,7 +7534,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="233" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" ht="16.5" thickBot="1">
       <c r="A233" t="s">
         <v>128</v>
       </c>
@@ -7564,7 +7563,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="234" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9" ht="16.5" thickBot="1">
       <c r="A234" t="s">
         <v>121</v>
       </c>
@@ -7593,7 +7592,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="235" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9" ht="16.5" thickBot="1">
       <c r="A235" t="s">
         <v>123</v>
       </c>
@@ -7622,7 +7621,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="236" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9" ht="16.5" thickBot="1">
       <c r="A236" t="s">
         <v>125</v>
       </c>
@@ -7658,16 +7657,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7678,7 +7677,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="16.5" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -7689,7 +7688,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="16.5" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -7700,7 +7699,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.5" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -7711,7 +7710,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="16.5" thickBot="1">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -7722,7 +7721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="16.5" thickBot="1">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -7733,7 +7732,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="16.5" thickBot="1">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -7744,7 +7743,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="16.5" thickBot="1">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -7755,7 +7754,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -7766,7 +7765,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="16.5" thickBot="1">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -7777,7 +7776,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="16.5" thickBot="1">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -7788,7 +7787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="16.5" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -7799,7 +7798,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="16.5" thickBot="1">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -7810,7 +7809,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -7821,7 +7820,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="16.5" thickBot="1">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -7832,7 +7831,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="16.5" thickBot="1">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -7843,7 +7842,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="16.5" thickBot="1">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -7854,7 +7853,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="16.5" thickBot="1">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -7865,7 +7864,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="16.5" thickBot="1">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -7876,7 +7875,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="16.5" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -7887,7 +7886,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="16.5" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
@@ -7898,7 +7897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -7909,7 +7908,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="16.5" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -7920,7 +7919,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="16.5" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
@@ -7931,7 +7930,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="16.5" thickBot="1">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
@@ -7942,7 +7941,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="16.5" thickBot="1">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
@@ -7953,7 +7952,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="16.5" thickBot="1">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
@@ -7964,7 +7963,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="16.5" thickBot="1">
       <c r="A28" s="1" t="s">
         <v>55</v>
       </c>
@@ -7975,7 +7974,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="16.5" thickBot="1">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -7986,7 +7985,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="16.5" thickBot="1">
       <c r="A30" s="1" t="s">
         <v>47</v>
       </c>
@@ -7997,7 +7996,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="16.5" thickBot="1">
       <c r="A31" s="1" t="s">
         <v>50</v>
       </c>
@@ -8008,7 +8007,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="16.5" thickBot="1">
       <c r="A32" s="1" t="s">
         <v>53</v>
       </c>
@@ -8019,7 +8018,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="16.5" thickBot="1">
       <c r="A33" s="1" t="s">
         <v>60</v>
       </c>
@@ -8030,7 +8029,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="16.5" thickBot="1">
       <c r="A34" s="1" t="s">
         <v>56</v>
       </c>
@@ -8041,7 +8040,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="16.5" thickBot="1">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -8052,7 +8051,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="16.5" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -8063,7 +8062,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="16.5" thickBot="1">
       <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
@@ -8074,7 +8073,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="16.5" thickBot="1">
       <c r="A38" s="1" t="s">
         <v>69</v>
       </c>
@@ -8085,7 +8084,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="16.5" thickBot="1">
       <c r="A39" s="1" t="s">
         <v>45</v>
       </c>
@@ -8096,7 +8095,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="16.5" thickBot="1">
       <c r="A40" s="1" t="s">
         <v>57</v>
       </c>
@@ -8107,7 +8106,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="16.5" thickBot="1">
       <c r="A41" s="1" t="s">
         <v>63</v>
       </c>
@@ -8118,7 +8117,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="16.5" thickBot="1">
       <c r="A42" s="1" t="s">
         <v>73</v>
       </c>
@@ -8129,7 +8128,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="16.5" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>75</v>
       </c>
@@ -8140,7 +8139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="16.5" thickBot="1">
       <c r="A44" s="1" t="s">
         <v>64</v>
       </c>
@@ -8151,7 +8150,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="16.5" thickBot="1">
       <c r="A45" s="1" t="s">
         <v>71</v>
       </c>
@@ -8162,7 +8161,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="16.5" thickBot="1">
       <c r="A46" s="1" t="s">
         <v>59</v>
       </c>
@@ -8173,7 +8172,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="16.5" thickBot="1">
       <c r="A47" s="1" t="s">
         <v>61</v>
       </c>
@@ -8184,7 +8183,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="16.5" thickBot="1">
       <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
@@ -8195,7 +8194,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="16.5" thickBot="1">
       <c r="A49" s="1" t="s">
         <v>84</v>
       </c>
@@ -8206,7 +8205,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="16.5" thickBot="1">
       <c r="A50" s="1" t="s">
         <v>87</v>
       </c>
@@ -8217,7 +8216,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="16.5" thickBot="1">
       <c r="A51" s="1" t="s">
         <v>77</v>
       </c>
@@ -8228,7 +8227,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="16.5" thickBot="1">
       <c r="A52" s="1" t="s">
         <v>79</v>
       </c>
@@ -8239,7 +8238,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="16.5" thickBot="1">
       <c r="A53" s="1" t="s">
         <v>70</v>
       </c>
@@ -8250,7 +8249,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="16.5" thickBot="1">
       <c r="A54" s="1" t="s">
         <v>92</v>
       </c>
@@ -8261,7 +8260,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="16.5" thickBot="1">
       <c r="A55" s="1" t="s">
         <v>88</v>
       </c>
@@ -8272,7 +8271,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="16.5" thickBot="1">
       <c r="A56" s="1" t="s">
         <v>90</v>
       </c>
@@ -8283,7 +8282,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="16.5" thickBot="1">
       <c r="A57" s="1" t="s">
         <v>80</v>
       </c>
@@ -8294,7 +8293,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="16.5" thickBot="1">
       <c r="A58" s="1" t="s">
         <v>82</v>
       </c>
@@ -8305,7 +8304,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="16.5" thickBot="1">
       <c r="A59" s="1" t="s">
         <v>85</v>
       </c>
@@ -8316,7 +8315,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="16.5" thickBot="1">
       <c r="A60" s="1" t="s">
         <v>98</v>
       </c>
@@ -8327,7 +8326,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="16.5" thickBot="1">
       <c r="A61" s="1" t="s">
         <v>67</v>
       </c>
@@ -8338,7 +8337,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="16.5" thickBot="1">
       <c r="A62" s="1" t="s">
         <v>91</v>
       </c>
@@ -8349,7 +8348,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="16.5" thickBot="1">
       <c r="A63" s="1" t="s">
         <v>94</v>
       </c>
@@ -8360,7 +8359,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="16.5" thickBot="1">
       <c r="A64" s="1" t="s">
         <v>105</v>
       </c>
@@ -8371,7 +8370,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="16.5" thickBot="1">
       <c r="A65" s="1" t="s">
         <v>96</v>
       </c>
@@ -8382,7 +8381,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="16.5" thickBot="1">
       <c r="A66" s="1" t="s">
         <v>97</v>
       </c>
@@ -8393,7 +8392,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="16.5" thickBot="1">
       <c r="A67" s="1" t="s">
         <v>108</v>
       </c>
@@ -8404,7 +8403,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="16.5" thickBot="1">
       <c r="A68" s="1" t="s">
         <v>99</v>
       </c>
@@ -8415,7 +8414,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="16.5" thickBot="1">
       <c r="A69" s="1" t="s">
         <v>111</v>
       </c>
@@ -8426,7 +8425,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="16.5" thickBot="1">
       <c r="A70" s="1" t="s">
         <v>107</v>
       </c>
@@ -8437,7 +8436,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="16.5" thickBot="1">
       <c r="A71" s="1" t="s">
         <v>110</v>
       </c>
@@ -8448,7 +8447,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="16.5" thickBot="1">
       <c r="A72" s="1" t="s">
         <v>106</v>
       </c>
@@ -8459,7 +8458,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="16.5" thickBot="1">
       <c r="A73" s="1" t="s">
         <v>115</v>
       </c>
@@ -8470,7 +8469,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="16.5" thickBot="1">
       <c r="A74" s="1" t="s">
         <v>119</v>
       </c>
@@ -8481,7 +8480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="16.5" thickBot="1">
       <c r="A75" s="1" t="s">
         <v>100</v>
       </c>
@@ -8492,7 +8491,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="16.5" thickBot="1">
       <c r="A76" s="1" t="s">
         <v>102</v>
       </c>
@@ -8503,7 +8502,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="16.5" thickBot="1">
       <c r="A77" s="1" t="s">
         <v>116</v>
       </c>
@@ -8514,7 +8513,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="16.5" thickBot="1">
       <c r="A78" s="1" t="s">
         <v>118</v>
       </c>
@@ -8525,7 +8524,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" ht="16.5" thickBot="1">
       <c r="A79" s="1" t="s">
         <v>113</v>
       </c>
@@ -8536,7 +8535,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" ht="16.5" thickBot="1">
       <c r="A80" s="1" t="s">
         <v>128</v>
       </c>
@@ -8547,7 +8546,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" ht="16.5" thickBot="1">
       <c r="A81" s="1" t="s">
         <v>121</v>
       </c>
@@ -8558,7 +8557,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" ht="16.5" thickBot="1">
       <c r="A82" s="1" t="s">
         <v>123</v>
       </c>
@@ -8569,7 +8568,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" ht="16.5" thickBot="1">
       <c r="A83" s="1" t="s">
         <v>125</v>
       </c>
@@ -8587,13 +8586,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>